<commit_message>
get cities and areas from an excel file
</commit_message>
<xml_diff>
--- a/includes/delivery.xlsx
+++ b/includes/delivery.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Workspace\Github\woocom\woocom\md-server\sources\woocom\wp-content\plugins\md-shipping-logic\includes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDCF6FF-0D6E-4CEC-BA17-1060257D1C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C326ED1-909E-4D40-872D-DAE17C4A4DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="178">
   <si>
     <t>city</t>
   </si>
@@ -108,6 +109,9 @@
     <t>Sacre Cœur</t>
   </si>
   <si>
+    <t xml:space="preserve">Patte D'oie </t>
+  </si>
+  <si>
     <t xml:space="preserve">Plateau </t>
   </si>
   <si>
@@ -129,9 +133,6 @@
     <t>Fann Amitié</t>
   </si>
   <si>
-    <t>HLM - Parcelle</t>
-  </si>
-  <si>
     <t>ngor</t>
   </si>
   <si>
@@ -180,29 +181,392 @@
     <t>plateau</t>
   </si>
   <si>
-    <t>hlm_parcelle</t>
-  </si>
-  <si>
-    <t>20:30</t>
-  </si>
-  <si>
     <t>2500</t>
   </si>
   <si>
-    <t xml:space="preserve">Patte D oie </t>
-  </si>
-  <si>
-    <t>19:30</t>
-  </si>
-  <si>
-    <t>21:00</t>
+    <t xml:space="preserve">Bel air </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dalifort </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camberene </t>
+  </si>
+  <si>
+    <t xml:space="preserve">thiaroye </t>
+  </si>
+  <si>
+    <t>Mbao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keur Massar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rufisque </t>
+  </si>
+  <si>
+    <t>parcelle_1_a_7</t>
+  </si>
+  <si>
+    <t>Parcelle 1 à 7</t>
+  </si>
+  <si>
+    <t>guediawaye</t>
+  </si>
+  <si>
+    <t>Guediawaye</t>
+  </si>
+  <si>
+    <t>Pikine</t>
+  </si>
+  <si>
+    <t>pikine</t>
+  </si>
+  <si>
+    <t>hann_marinas</t>
+  </si>
+  <si>
+    <t>bel_air</t>
+  </si>
+  <si>
+    <t>dalifort</t>
+  </si>
+  <si>
+    <t>camberene</t>
+  </si>
+  <si>
+    <t>keur_mbaye_fall</t>
+  </si>
+  <si>
+    <t>mbao</t>
+  </si>
+  <si>
+    <t>keur_massar</t>
+  </si>
+  <si>
+    <t>rufisque</t>
+  </si>
+  <si>
+    <t>Thiaroye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keur Mbaye Fall </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hann Marinas </t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>14:00</t>
+  </si>
+  <si>
+    <t>4000</t>
+  </si>
+  <si>
+    <t>hann</t>
+  </si>
+  <si>
+    <t>Hann</t>
+  </si>
+  <si>
+    <t>foire</t>
+  </si>
+  <si>
+    <t>Foire</t>
+  </si>
+  <si>
+    <t>parcelles_assainies</t>
+  </si>
+  <si>
+    <t>Parcelles Assainies</t>
+  </si>
+  <si>
+    <t>ouakam</t>
+  </si>
+  <si>
+    <t>Ouakam</t>
+  </si>
+  <si>
+    <t>18:30</t>
+  </si>
+  <si>
+    <t>3500</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>Koumassi</t>
+  </si>
+  <si>
+    <t>Faya</t>
+  </si>
+  <si>
+    <t>Plateau</t>
+  </si>
+  <si>
+    <t>Angre</t>
+  </si>
+  <si>
+    <t>Marcory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treicheville </t>
+  </si>
+  <si>
+    <t>Port Bouet</t>
+  </si>
+  <si>
+    <t>Abobo Gare / Sud</t>
+  </si>
+  <si>
+    <t>Yopougon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yopougon </t>
+  </si>
+  <si>
+    <t>18:00</t>
+  </si>
+  <si>
+    <t>koumassi</t>
+  </si>
+  <si>
+    <t>faya</t>
+  </si>
+  <si>
+    <t>angre</t>
+  </si>
+  <si>
+    <t>marcory</t>
+  </si>
+  <si>
+    <t>treichville</t>
+  </si>
+  <si>
+    <t>port_bouet</t>
+  </si>
+  <si>
+    <t>abobo_gare_sud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bassam </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agnama </t>
+  </si>
+  <si>
+    <t>Vridi cité</t>
+  </si>
+  <si>
+    <t>Port Bouet Anani</t>
+  </si>
+  <si>
+    <t>port_bouet_anani</t>
+  </si>
+  <si>
+    <t>yopougon_pk17</t>
+  </si>
+  <si>
+    <t>Yopougon PK17</t>
+  </si>
+  <si>
+    <t>bassam</t>
+  </si>
+  <si>
+    <t>abobo_pk18</t>
+  </si>
+  <si>
+    <t>Abobo PK18</t>
+  </si>
+  <si>
+    <t>abobo_belleville</t>
+  </si>
+  <si>
+    <t>agnama</t>
+  </si>
+  <si>
+    <t>vridi_cite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abobo Belle-ville </t>
+  </si>
+  <si>
+    <t>abobo_ndotre</t>
+  </si>
+  <si>
+    <t>Abobo Ndotré</t>
+  </si>
+  <si>
+    <t>attoban</t>
+  </si>
+  <si>
+    <t>Attoban</t>
+  </si>
+  <si>
+    <t>bingerville_devant_lycee_garcon</t>
+  </si>
+  <si>
+    <t>bingerville_derriere_lycee_garcon</t>
+  </si>
+  <si>
+    <t>Bingerville – Devant lycée garçon</t>
+  </si>
+  <si>
+    <t>Bingerville – Derrière lycée garçon</t>
+  </si>
+  <si>
+    <t>bietry</t>
+  </si>
+  <si>
+    <t>remblais</t>
+  </si>
+  <si>
+    <t>cite_cicogi</t>
+  </si>
+  <si>
+    <t>adjame</t>
+  </si>
+  <si>
+    <t>Adjamé</t>
+  </si>
+  <si>
+    <t>Remblais</t>
+  </si>
+  <si>
+    <t>Bietry</t>
+  </si>
+  <si>
+    <t>Cité CICOGI</t>
+  </si>
+  <si>
+    <t>riviera_3_4</t>
+  </si>
+  <si>
+    <t>riviera_1_2</t>
+  </si>
+  <si>
+    <t>Riviera 1 – 2</t>
+  </si>
+  <si>
+    <t>Riviéra 3 – 4</t>
+  </si>
+  <si>
+    <t>riviera_5_6</t>
+  </si>
+  <si>
+    <t>Riviéra 5 – 6</t>
+  </si>
+  <si>
+    <t>libreville</t>
+  </si>
+  <si>
+    <t>akanda</t>
+  </si>
+  <si>
+    <t>owendo</t>
+  </si>
+  <si>
+    <t>mindoumbe</t>
+  </si>
+  <si>
+    <t>bikele</t>
+  </si>
+  <si>
+    <t>premier campement</t>
+  </si>
+  <si>
+    <t>Akanda</t>
+  </si>
+  <si>
+    <t>Owendo</t>
+  </si>
+  <si>
+    <t>Mindoumbe</t>
+  </si>
+  <si>
+    <t>Bikele</t>
+  </si>
+  <si>
+    <t>Premier Campement</t>
+  </si>
+  <si>
+    <t>Show message :  If you were delivering in Abidjan city (zones gratuites), you could have free delivery and receive your item today !</t>
+  </si>
+  <si>
+    <t>Show message :  If you were delivering in Dakar city, you could have free delivery and receive your item today !</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>city_name</t>
+  </si>
+  <si>
+    <t>sn</t>
+  </si>
+  <si>
+    <t>Thiès</t>
+  </si>
+  <si>
+    <t>thies</t>
+  </si>
+  <si>
+    <t>saly</t>
+  </si>
+  <si>
+    <t>Saly</t>
+  </si>
+  <si>
+    <t>mbour</t>
+  </si>
+  <si>
+    <t>Mbour</t>
+  </si>
+  <si>
+    <t>saint louis</t>
+  </si>
+  <si>
+    <t>Saint Louis</t>
+  </si>
+  <si>
+    <t>ga</t>
+  </si>
+  <si>
+    <t>Libreville</t>
+  </si>
+  <si>
+    <t>dakar_banlieue</t>
+  </si>
+  <si>
+    <t>Dakar (Livraison Gratuit)</t>
+  </si>
+  <si>
+    <t>Dakar (Livraison Payante)</t>
+  </si>
+  <si>
+    <t>abidjan_zones_gratuites</t>
+  </si>
+  <si>
+    <t>abidjaabidjan_zones_payantes</t>
+  </si>
+  <si>
+    <t>ci</t>
+  </si>
+  <si>
+    <t>Abidjan (Livraison Gratuite)</t>
+  </si>
+  <si>
+    <t>Abidjan (Livraison Payante)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,13 +574,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -231,8 +614,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -513,25 +911,573 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B4C38E-611D-4CFF-9B0A-26F9D95E9F67}">
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="11">
+        <v>2000</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="11">
+        <v>7000</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="11">
+        <v>3000</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2000</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1">
+        <v>7000</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="1">
+        <v>3000</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="1">
+        <v>7000</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="1">
+        <v>3000</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="1">
+        <v>3000</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="1">
+        <v>7000</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="1">
+        <v>3000</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" s="1">
+        <v>7000</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="1">
+        <v>3000</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="1">
+        <v>3000</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="1">
+        <v>3000</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="1">
+        <v>3000</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="1">
+        <v>3500</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B13" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="1">
+        <v>4000</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B14" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="1">
+        <v>5000</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="12">
+        <v>2000</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="12">
+        <v>7000</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" s="12">
+        <v>3000</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="12">
+        <v>2000</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="12">
+        <v>7000</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" s="12">
+        <v>3000</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:T65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScale="99" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="1"/>
-    <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" style="1" customWidth="1"/>
-    <col min="4" max="6" width="8.77734375" style="1"/>
-    <col min="7" max="7" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.77734375" style="1"/>
+    <col min="1" max="1" width="26.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="109.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -556,7 +1502,7 @@
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -583,7 +1529,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>12</v>
@@ -591,7 +1537,7 @@
       <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -601,7 +1547,7 @@
         <v>14</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -626,7 +1572,7 @@
       <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -636,7 +1582,7 @@
         <v>14</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -661,7 +1607,7 @@
       <c r="G4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -671,7 +1617,7 @@
         <v>14</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -682,7 +1628,7 @@
         <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
@@ -696,7 +1642,7 @@
       <c r="G5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -706,7 +1652,7 @@
         <v>14</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -717,7 +1663,7 @@
         <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
@@ -731,7 +1677,7 @@
       <c r="G6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -741,7 +1687,7 @@
         <v>14</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -752,7 +1698,7 @@
         <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>10</v>
@@ -766,7 +1712,7 @@
       <c r="G7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -776,7 +1722,7 @@
         <v>14</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -787,7 +1733,7 @@
         <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>10</v>
@@ -801,7 +1747,7 @@
       <c r="G8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -811,7 +1757,7 @@
         <v>14</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -822,7 +1768,7 @@
         <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>10</v>
@@ -836,7 +1782,7 @@
       <c r="G9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -846,7 +1792,7 @@
         <v>14</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -871,7 +1817,7 @@
       <c r="G10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -881,7 +1827,7 @@
         <v>14</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -906,7 +1852,7 @@
       <c r="G11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -916,7 +1862,7 @@
         <v>14</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -941,7 +1887,7 @@
       <c r="G12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -951,7 +1897,7 @@
         <v>14</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -976,7 +1922,7 @@
       <c r="G13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -986,7 +1932,7 @@
         <v>14</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -997,7 +1943,7 @@
         <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>10</v>
@@ -1011,7 +1957,7 @@
       <c r="G14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -1021,7 +1967,7 @@
         <v>14</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1046,7 +1992,7 @@
       <c r="G15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I15" s="1" t="s">
@@ -1056,7 +2002,7 @@
         <v>14</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>52</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1076,12 +2022,12 @@
         <v>11</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -1091,10 +2037,10 @@
         <v>14</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -1102,7 +2048,7 @@
         <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>10</v>
@@ -1111,12 +2057,12 @@
         <v>11</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I17" s="1" t="s">
@@ -1126,10 +2072,10 @@
         <v>14</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -1137,7 +2083,7 @@
         <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>10</v>
@@ -1146,12 +2092,12 @@
         <v>11</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I18" s="1" t="s">
@@ -1161,18 +2107,18 @@
         <v>14</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>10</v>
@@ -1181,12 +2127,12 @@
         <v>11</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I19" s="1" t="s">
@@ -1196,10 +2142,1413 @@
         <v>14</v>
       </c>
       <c r="K19" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" t="s">
         <v>52</v>
       </c>
+      <c r="D21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" s="2">
+        <v>2000</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M26" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="T26" s="2"/>
+    </row>
+    <row r="27" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F27" s="2">
+        <v>2500</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L27" s="2"/>
+      <c r="M27" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="T27" s="2"/>
+    </row>
+    <row r="28" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F28" s="2">
+        <v>2500</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L28" s="2"/>
+      <c r="M28" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="T28" s="2"/>
+    </row>
+    <row r="29" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F29" s="2">
+        <v>2500</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L29" s="2"/>
+      <c r="M29" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="T29" s="2"/>
+    </row>
+    <row r="30" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F30" s="2">
+        <v>2500</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L30" s="2"/>
+      <c r="M30" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="T30" s="2"/>
+    </row>
+    <row r="31" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F31" s="2">
+        <v>3500</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L31" s="2"/>
+      <c r="M31" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="T31" s="2"/>
+    </row>
+    <row r="32" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F32" s="2">
+        <v>3500</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L32" s="2"/>
+      <c r="M32" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="T32" s="2"/>
+    </row>
+    <row r="33" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33" s="2">
+        <v>3500</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L33" s="2"/>
+      <c r="M33" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="T33" s="2"/>
+    </row>
+    <row r="34" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F34" s="2">
+        <v>4500</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L34" s="2"/>
+      <c r="M34" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="T34" s="2"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A35" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A36" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B36" t="s">
+        <v>138</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A37" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B37" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37" t="s">
+        <v>140</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A38" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B38" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A39" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A40" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B40" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A41" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B41" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A42" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B42" t="s">
+        <v>105</v>
+      </c>
+      <c r="C42" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A43" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B43" t="s">
+        <v>106</v>
+      </c>
+      <c r="C43" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A44" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B44" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" t="s">
+        <v>97</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A45" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J45" s="6"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A46" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J46" s="6"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A47" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B47" t="s">
+        <v>133</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A48" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B48" t="s">
+        <v>131</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B49" t="s">
+        <v>130</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B50" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B51" t="s">
+        <v>142</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H51" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J51" s="6"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A52" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B52" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" t="s">
+        <v>98</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H52" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B53" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" t="s">
+        <v>90</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A54" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H54" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M54" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A55" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M55" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A56" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H56" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M56" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A57" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H57" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M57" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A58" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H58" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M58" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A59" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H59" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M59" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A60" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H60" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M60" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A61" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H61" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M61" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A62" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H62" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M62" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L63"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L64"/>
+    </row>
+    <row r="65" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L65"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>